<commit_message>
Created TableRow and TableCell components
</commit_message>
<xml_diff>
--- a/Prop destinations.xlsx
+++ b/Prop destinations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Prop</t>
   </si>
@@ -136,16 +136,13 @@
     <t xml:space="preserve">6 - SelectionRect</t>
   </si>
   <si>
-    <t>tbodyRef</t>
+    <t>tableBodyRef</t>
   </si>
   <si>
     <t>selectionRect</t>
   </si>
   <si>
     <t>dragSelectStart</t>
-  </si>
-  <si>
-    <t>rows</t>
   </si>
   <si>
     <t>columnResizeStart</t>
@@ -188,7 +185,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -203,12 +200,18 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <color theme="1"/>
       <sz val="14"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,6 +224,12 @@
         <bgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -231,22 +240,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -317,7 +329,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>890585</xdr:colOff>
+      <xdr:colOff>890584</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>685798</xdr:rowOff>
     </xdr:from>
@@ -1687,6 +1699,9 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1812,8 +1827,14 @@
       <c r="C24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" t="s">
         <v>39</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="25" ht="14.25">
@@ -1823,8 +1844,8 @@
       <c r="B25" t="s">
         <v>27</v>
       </c>
-      <c r="C25" t="s">
-        <v>19</v>
+      <c r="C25" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" s="3" customFormat="1" ht="14.25">
@@ -1854,23 +1875,13 @@
         <v>43</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" ht="14.25">
-      <c r="A29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="2" t="s">
         <v>18</v>
       </c>
     </row>
+    <row r="29" ht="14.25"/>
     <row r="36" ht="14.25"/>
     <row r="37" ht="14.25">
       <c r="A37" s="2"/>
@@ -1896,82 +1907,82 @@
     <col min="7" max="16384" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
+    <row r="1" s="5" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" s="5" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" s="4" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" s="5" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" s="4" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" s="5" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" s="4" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" s="5" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" s="4" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" s="5" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" s="4" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="4"/>
+      <c r="G6" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Moved row event handlers inside TableRow
</commit_message>
<xml_diff>
--- a/Prop destinations.xlsx
+++ b/Prop destinations.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Props" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Prop</t>
   </si>
@@ -79,6 +79,9 @@
     <t xml:space="preserve">6 - ColumnGroup</t>
   </si>
   <si>
+    <t xml:space="preserve">7 - TableRow</t>
+  </si>
+  <si>
     <t>className</t>
   </si>
   <si>
@@ -169,7 +172,7 @@
     <t>BodyContainer</t>
   </si>
   <si>
-    <t>ColumnResizer</t>
+    <t>ColumnGroup</t>
   </si>
   <si>
     <t>TableHead</t>
@@ -179,13 +182,22 @@
   </si>
   <si>
     <t>TableBody</t>
+  </si>
+  <si>
+    <t>TableHeader</t>
+  </si>
+  <si>
+    <t>TableRow</t>
+  </si>
+  <si>
+    <t>TableCell</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="13">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -210,8 +222,61 @@
       <sz val="14"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <color theme="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <color theme="1"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <color theme="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b/>
+      <color theme="1"/>
+      <sz val="10"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b/>
+      <color rgb="FF00B050"/>
+      <sz val="10"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b/>
+      <color rgb="FF7030A0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b/>
+      <color theme="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b/>
+      <color theme="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b/>
+      <color rgb="FF00B050"/>
+      <sz val="10"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,12 +295,42 @@
         <bgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill/>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dotted">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color theme="1"/>
+      </top>
+      <bottom style="dotted">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color theme="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -245,13 +340,64 @@
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="25">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="5" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="6" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="4" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="5" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="6" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="7" fillId="4" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="8" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="7" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="9" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="10" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="11" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="12" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="4" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="5" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="6" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="11" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -269,16 +415,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>714374</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>714372</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>666749</xdr:rowOff>
+      <xdr:rowOff>657222</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>714374</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>714372</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>228599</xdr:rowOff>
+      <xdr:rowOff>219071</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -290,7 +436,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="6391274" y="4248149"/>
+          <a:off x="7038972" y="4238622"/>
           <a:ext cx="0" cy="457199"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -298,9 +444,7 @@
         </a:prstGeom>
         <a:ln w="19049" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+            <a:srgbClr val="43739E"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter/>
@@ -328,16 +472,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>890584</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>890583</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>685798</xdr:rowOff>
+      <xdr:rowOff>676271</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>623886</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>623882</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>266698</xdr:rowOff>
+      <xdr:rowOff>257170</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -349,7 +493,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="5148261" y="1581148"/>
+          <a:off x="5795958" y="1571621"/>
           <a:ext cx="1152524" cy="476249"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -387,16 +531,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>828673</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>828671</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>685798</xdr:rowOff>
+      <xdr:rowOff>676271</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>561972</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>561969</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>266698</xdr:rowOff>
+      <xdr:rowOff>257170</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -408,7 +552,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1" flipV="0">
-          <a:off x="2247898" y="3371848"/>
+          <a:off x="2895596" y="3362321"/>
           <a:ext cx="1152523" cy="476249"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -446,16 +590,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>857249</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>857247</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>666749</xdr:rowOff>
+      <xdr:rowOff>657222</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>590547</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>590544</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>247648</xdr:rowOff>
+      <xdr:rowOff>238120</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -467,7 +611,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1" flipV="0">
-          <a:off x="5114923" y="4248149"/>
+          <a:off x="5762622" y="4238622"/>
           <a:ext cx="1152522" cy="476248"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -505,16 +649,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>700086</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>700084</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>685798</xdr:rowOff>
+      <xdr:rowOff>676271</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>700086</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>700084</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>247647</xdr:rowOff>
+      <xdr:rowOff>238119</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -526,7 +670,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="4957761" y="685798"/>
+          <a:off x="5605459" y="676271"/>
           <a:ext cx="0" cy="457198"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -564,16 +708,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>695323</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>695321</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>685799</xdr:rowOff>
+      <xdr:rowOff>676272</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>695323</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>695321</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>247648</xdr:rowOff>
+      <xdr:rowOff>238120</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -585,7 +729,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="3533773" y="2476499"/>
+          <a:off x="4181471" y="2466972"/>
           <a:ext cx="0" cy="457198"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -623,16 +767,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>857249</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>857247</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>666749</xdr:rowOff>
+      <xdr:rowOff>657222</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>590548</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590545</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>247649</xdr:rowOff>
+      <xdr:rowOff>238121</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -644,7 +788,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="6534149" y="4248149"/>
+          <a:off x="7181847" y="4238622"/>
           <a:ext cx="1152523" cy="476249"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -682,16 +826,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>823911</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>823909</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>685798</xdr:rowOff>
+      <xdr:rowOff>676271</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>557209</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>557206</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>266697</xdr:rowOff>
+      <xdr:rowOff>257169</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -703,7 +847,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1" flipV="0">
-          <a:off x="3662360" y="1581148"/>
+          <a:off x="4310059" y="1571621"/>
           <a:ext cx="1152522" cy="476248"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -741,16 +885,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>904873</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>904871</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>685798</xdr:rowOff>
+      <xdr:rowOff>676271</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>533399</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>533396</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>276223</xdr:rowOff>
+      <xdr:rowOff>266696</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -762,7 +906,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="3743323" y="3371848"/>
+          <a:off x="4391021" y="3362321"/>
           <a:ext cx="2466975" cy="485775"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -800,16 +944,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>704848</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>704846</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>685799</xdr:rowOff>
+      <xdr:rowOff>676272</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>704848</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>704846</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>247647</xdr:rowOff>
+      <xdr:rowOff>238119</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -821,7 +965,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="6381748" y="2476499"/>
+          <a:off x="7029446" y="2466972"/>
           <a:ext cx="0" cy="457197"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -859,16 +1003,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>719136</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>719134</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>676273</xdr:rowOff>
+      <xdr:rowOff>666746</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>719136</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>719134</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>238122</xdr:rowOff>
+      <xdr:rowOff>228594</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -880,7 +1024,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="4976811" y="1571623"/>
+          <a:off x="5624509" y="1562096"/>
           <a:ext cx="0" cy="457198"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -918,16 +1062,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>842961</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>842959</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>647699</xdr:rowOff>
+      <xdr:rowOff>638172</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>576258</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>576256</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>228599</xdr:rowOff>
+      <xdr:rowOff>219070</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -939,7 +1083,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1" flipV="0">
-          <a:off x="842961" y="4229100"/>
+          <a:off x="1490659" y="4219572"/>
           <a:ext cx="1152522" cy="476248"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -977,16 +1121,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>842961</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>842959</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>647699</xdr:rowOff>
+      <xdr:rowOff>638172</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>576259</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>576257</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
+      <xdr:rowOff>219071</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -998,8 +1142,185 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="2262186" y="4229100"/>
+          <a:off x="2909884" y="4219572"/>
           <a:ext cx="1152523" cy="476249"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19049" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter/>
+          <a:tailEnd type="arrow" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>714373</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>685798</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>714373</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>247646</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="" hidden="0"/>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+        </xdr:cNvCxnSpPr>
+        <xdr:nvPr isPhoto="0" userDrawn="0"/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="8458198" y="6057898"/>
+          <a:ext cx="0" cy="457198"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19049" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter/>
+          <a:tailEnd type="arrow" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>714373</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>647698</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>714373</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>209546</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="" hidden="0"/>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+        </xdr:cNvCxnSpPr>
+        <xdr:nvPr isPhoto="0" userDrawn="0"/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="8458198" y="5124448"/>
+          <a:ext cx="0" cy="457198"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19049" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter/>
+          <a:tailEnd type="arrow" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>742946</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>657224</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>742946</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>219072</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="" hidden="0"/>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+        </xdr:cNvCxnSpPr>
+        <xdr:nvPr isPhoto="0" userDrawn="0"/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="4229096" y="5133974"/>
+          <a:ext cx="0" cy="457198"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1629,28 +1950,31 @@
       <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
       </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
@@ -1659,7 +1983,7 @@
     </row>
     <row r="11" ht="14.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
@@ -1668,25 +1992,25 @@
     </row>
     <row r="12" ht="14.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
@@ -1695,19 +2019,19 @@
     </row>
     <row r="15" ht="14.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
@@ -1716,7 +2040,7 @@
     </row>
     <row r="17" ht="14.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
@@ -1725,16 +2049,16 @@
     </row>
     <row r="18" ht="14.25">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
@@ -1743,7 +2067,7 @@
     </row>
     <row r="20" ht="14.25">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -1766,25 +2090,25 @@
     </row>
     <row r="21" ht="14.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>19</v>
+      <c r="G21" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22" ht="14.25">
@@ -1798,40 +2122,41 @@
         <v>18</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" s="4" customFormat="1" ht="14.25">
+      <c r="A23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" s="3" customFormat="1" ht="14.25">
-      <c r="A23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
     </row>
     <row r="24" ht="14.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>23</v>
+      <c r="D24" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>19</v>
@@ -1839,40 +2164,40 @@
     </row>
     <row r="25" ht="14.25">
       <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" s="4" customFormat="1" ht="14.25">
+      <c r="A26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="B25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" s="3" customFormat="1" ht="14.25">
-      <c r="A26" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="27" ht="14.25">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" ht="14.25">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>10</v>
@@ -1896,98 +2221,149 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="1"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="6" width="21.28125"/>
-    <col min="7" max="16384" width="9.140625"/>
+    <col customWidth="1" min="1" max="1" style="7" width="9.7109375"/>
+    <col customWidth="1" min="2" max="7" style="6" width="21.28125"/>
+    <col min="8" max="16384" style="6" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" s="5" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+    <row r="1" s="8" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A1" s="9">
+        <v>1</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" s="5" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" s="11" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A2" s="12">
+        <v>2</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" s="11" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A3" s="12">
+        <v>3</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" s="5" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5" t="s">
+      <c r="F3" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" s="11" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A4" s="12">
+        <v>4</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" s="5" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
+      <c r="G4" s="13"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" s="11" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A5" s="12">
+        <v>5</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" s="5" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A6" s="5" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" s="11" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A6" s="12">
+        <v>6</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="E6" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="F6" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" s="11" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A7" s="12">
+        <v>7</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" s="21" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A8" s="22">
+        <v>8</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="24" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="landscape" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <pageMargins left="0.25196850393700787" right="0.25196850393700787" top="0.25196850393700787" bottom="0.25196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="landscape" pageOrder="downThenOver" paperSize="9" scale="96" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Combined dragSelection, lastMousePos, lastRelMouseY and origin into dragSelection
</commit_message>
<xml_diff>
--- a/Prop destinations.xlsx
+++ b/Prop destinations.xlsx
@@ -157,7 +157,7 @@
     <t>setResizing</t>
   </si>
   <si>
-    <t>touchingIndex</t>
+    <t>isTouching</t>
   </si>
   <si>
     <t>Connector</t>
@@ -206,7 +206,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -265,12 +265,6 @@
       <b/>
       <color rgb="FF7030A0"/>
       <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <b/>
-      <color theme="1"/>
-      <sz val="11"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -349,7 +343,7 @@
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
@@ -394,9 +388,6 @@
     <xf fontId="11" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="12" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="4" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -406,7 +397,7 @@
     <xf fontId="6" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="11" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="10" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -483,16 +474,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>828671</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>676271</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>866774</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>666747</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>561969</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>257170</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600071</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>247645</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -504,66 +495,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1" flipV="0">
-          <a:off x="2895596" y="3362321"/>
-          <a:ext cx="1152523" cy="476249"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19049" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter/>
-          <a:tailEnd type="arrow" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>857247</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>657222</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>590544</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>238120</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="" hidden="0"/>
-        <xdr:cNvCxnSpPr>
-          <a:cxnSpLocks/>
-        </xdr:cNvCxnSpPr>
-        <xdr:nvPr isPhoto="0" userDrawn="0"/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipH="1" flipV="0">
-          <a:off x="5762622" y="4238622"/>
+          <a:off x="7191374" y="4248147"/>
           <a:ext cx="1152522" cy="476248"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -614,7 +546,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="" hidden="0"/>
+        <xdr:cNvPr id="6" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -660,20 +592,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>695321</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>700084</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>676272</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>695321</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>700084</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>238120</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="8" name="" hidden="0"/>
+        <xdr:cNvPr id="7" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -681,7 +613,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="4181471" y="2466972"/>
+          <a:off x="5605459" y="2466972"/>
           <a:ext cx="0" cy="457198"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -719,20 +651,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>857247</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>866774</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>657222</xdr:rowOff>
+      <xdr:rowOff>666747</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>590545</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600072</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>238121</xdr:rowOff>
+      <xdr:rowOff>247646</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="" hidden="0"/>
+        <xdr:cNvPr id="8" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -740,7 +672,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="7181847" y="4238622"/>
+          <a:off x="8610599" y="4248147"/>
           <a:ext cx="1152523" cy="476249"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -791,7 +723,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="" hidden="0"/>
+        <xdr:cNvPr id="9" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -837,20 +769,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>904871</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>809620</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>676271</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>533396</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>438145</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>266696</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="11" name="" hidden="0"/>
+        <xdr:cNvPr id="10" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -858,7 +790,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="4391021" y="3362321"/>
+          <a:off x="5714995" y="3362321"/>
           <a:ext cx="2466975" cy="485775"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -909,7 +841,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="12" name="" hidden="0"/>
+        <xdr:cNvPr id="11" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -968,7 +900,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="" hidden="0"/>
+        <xdr:cNvPr id="12" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1027,7 +959,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="" hidden="0"/>
+        <xdr:cNvPr id="13" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1086,7 +1018,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="" hidden="0"/>
+        <xdr:cNvPr id="14" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1132,20 +1064,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>714373</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>685798</xdr:rowOff>
+      <xdr:rowOff>695323</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>714373</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>247646</xdr:rowOff>
+      <xdr:rowOff>257171</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="" hidden="0"/>
+        <xdr:cNvPr id="15" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1153,7 +1085,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="8458198" y="6057898"/>
+          <a:off x="9886950" y="6067423"/>
           <a:ext cx="0" cy="457198"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1191,20 +1123,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>714373</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>647698</xdr:rowOff>
+      <xdr:rowOff>657223</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>714373</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>209546</xdr:rowOff>
+      <xdr:rowOff>219071</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="" hidden="0"/>
+        <xdr:cNvPr id="16" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1212,7 +1144,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="8458198" y="5124448"/>
+          <a:off x="9886950" y="5133973"/>
           <a:ext cx="0" cy="457198"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1263,7 +1195,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="18" name="" hidden="0"/>
+        <xdr:cNvPr id="17" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1309,16 +1241,75 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>704846</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>714373</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>657222</xdr:rowOff>
+      <xdr:rowOff>666747</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>704846</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>714373</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>219070</xdr:rowOff>
+      <xdr:rowOff>228595</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="" hidden="0"/>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+        </xdr:cNvCxnSpPr>
+        <xdr:nvPr isPhoto="0" userDrawn="0"/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="8458198" y="4248147"/>
+          <a:ext cx="0" cy="457197"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19049" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter/>
+          <a:tailEnd type="arrow" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>928682</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>676271</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>557206</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>266695</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -1329,9 +1320,9 @@
         <xdr:nvPr isPhoto="0" userDrawn="0"/>
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
-        <a:xfrm flipH="0" flipV="0">
-          <a:off x="7029446" y="4238622"/>
-          <a:ext cx="0" cy="457197"/>
+        <a:xfrm flipH="1" flipV="0">
+          <a:off x="2995607" y="3362321"/>
+          <a:ext cx="2466973" cy="485773"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2140,18 +2131,18 @@
       </c>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" s="4" customFormat="1" ht="14.25">
+    <row r="23" s="2" customFormat="1" ht="14.25">
       <c r="A23" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" ht="14.25">
       <c r="A24" s="5" t="s">
@@ -2184,14 +2175,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" s="4" customFormat="1" ht="14.25">
+    <row r="26" s="2" customFormat="1" ht="14.25">
       <c r="A26" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2202,8 +2193,11 @@
       <c r="B27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="3" t="s">
         <v>24</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="28" ht="14.25">
@@ -2233,9 +2227,9 @@
         <v>47</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2265,8 +2259,8 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" style="7" width="9.7109375"/>
-    <col customWidth="1" min="2" max="7" style="6" width="21.28125"/>
-    <col min="8" max="16384" style="6" width="9.140625"/>
+    <col customWidth="1" min="2" max="8" style="6" width="21.28125"/>
+    <col min="9" max="16384" style="6" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="1" ht="70.5" customHeight="1">
@@ -2281,6 +2275,7 @@
       </c>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="2" s="11" customFormat="1" ht="70.5" customHeight="1">
       <c r="A2" s="12">
@@ -2294,23 +2289,25 @@
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" s="11" customFormat="1" ht="70.5" customHeight="1">
       <c r="A3" s="12">
         <v>3</v>
       </c>
       <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="15" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>50</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>11</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>51</v>
       </c>
       <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" s="11" customFormat="1" ht="70.5" customHeight="1">
       <c r="A4" s="12">
@@ -2318,30 +2315,29 @@
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="13"/>
       <c r="F4" s="13" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="13"/>
-      <c r="H4" s="18"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" s="11" customFormat="1" ht="70.5" customHeight="1">
       <c r="A5" s="12">
         <v>5</v>
       </c>
       <c r="B5" s="13"/>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>53</v>
       </c>
       <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="13"/>
+      <c r="G5" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" s="11" customFormat="1" ht="70.5" customHeight="1">
       <c r="A6" s="12">
@@ -2354,13 +2350,13 @@
       <c r="D6" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="F6" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="G6" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="H6" s="16" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2370,32 +2366,32 @@
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="13"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="13"/>
+      <c r="H7" s="18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" s="21" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A8" s="22">
+    <row r="8" s="20" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A8" s="21">
         <v>8</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.25196850393700787" right="0.25196850393700787" top="0.25196850393700787" bottom="0.25196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="landscape" pageOrder="downThenOver" paperSize="9" scale="96" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="landscape" pageOrder="downThenOver" paperSize="9" scale="94" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added automatic scrolling when resizing headers
</commit_message>
<xml_diff>
--- a/Prop destinations.xlsx
+++ b/Prop destinations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Prop</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>isTouching</t>
+  </si>
+  <si>
+    <t>scrollToPos</t>
   </si>
   <si>
     <t>Connector</t>
@@ -347,9 +350,9 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -424,7 +427,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>623882</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>257170</xdr:rowOff>
+      <xdr:rowOff>257169</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -778,7 +781,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>438145</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>266696</xdr:rowOff>
+      <xdr:rowOff>266695</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -2106,10 +2109,10 @@
       <c r="E21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2132,10 +2135,10 @@
       <c r="F22" s="2"/>
     </row>
     <row r="23" s="2" customFormat="1" ht="14.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -2145,7 +2148,7 @@
       <c r="E23" s="2"/>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B24" t="s">
@@ -2154,7 +2157,7 @@
       <c r="C24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E24" t="s">
@@ -2165,21 +2168,21 @@
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" s="2" customFormat="1" ht="14.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -2193,7 +2196,7 @@
       <c r="B27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -2207,7 +2210,7 @@
       <c r="B28" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2215,22 +2218,33 @@
       <c r="A29" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>18</v>
+      <c r="B29" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="36" ht="14.25"/>
@@ -2271,7 +2285,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
@@ -2285,7 +2299,7 @@
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -2301,10 +2315,10 @@
         <v>11</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
@@ -2316,7 +2330,7 @@
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
       <c r="E4" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>13</v>
@@ -2330,12 +2344,12 @@
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H5" s="13"/>
     </row>
@@ -2344,20 +2358,20 @@
         <v>6</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>55</v>
-      </c>
       <c r="H6" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" s="11" customFormat="1" ht="70.5" customHeight="1">
@@ -2367,12 +2381,12 @@
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" s="20" customFormat="1" ht="70.5" customHeight="1">
@@ -2385,7 +2399,7 @@
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
       <c r="H8" s="23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added back keyboard navigation
</commit_message>
<xml_diff>
--- a/Prop destinations.xlsx
+++ b/Prop destinations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Prop</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>onKeyDown</t>
-  </si>
-  <si>
-    <t>liveColumnResize</t>
   </si>
   <si>
     <t>options</t>
@@ -346,13 +343,12 @@
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2058,16 +2054,33 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
       <c r="C19" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" ht="14.25">
@@ -2075,118 +2088,109 @@
         <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" ht="14.25">
       <c r="A21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" s="2" customFormat="1" ht="14.25">
+      <c r="A22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" ht="14.25">
-      <c r="A22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" s="2" customFormat="1" ht="14.25">
-      <c r="A23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="24" ht="14.25">
       <c r="A24" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E24" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" ht="14.25">
-      <c r="A25" s="4" t="s">
+    </row>
+    <row r="25" s="2" customFormat="1" ht="14.25">
+      <c r="A25" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" s="2" customFormat="1" ht="14.25">
-      <c r="A26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>41</v>
+      <c r="D26" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="27" ht="14.25">
@@ -2194,13 +2198,10 @@
         <v>44</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" ht="14.25">
@@ -2208,48 +2209,37 @@
         <v>45</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" t="s">
+      <c r="A29" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" ht="14.25">
-      <c r="A30" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" ht="14.25">
-      <c r="A31" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" ht="14.25"/>
-    <row r="37" ht="14.25">
-      <c r="A37" s="2"/>
+    <row r="35" ht="14.25"/>
+    <row r="36" ht="14.25">
+      <c r="A36" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -2272,134 +2262,134 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" style="7" width="9.7109375"/>
-    <col customWidth="1" min="2" max="8" style="6" width="21.28125"/>
-    <col min="9" max="16384" style="6" width="9.140625"/>
+    <col customWidth="1" min="1" max="1" style="6" width="9.7109375"/>
+    <col customWidth="1" min="2" max="8" style="5" width="21.28125"/>
+    <col min="9" max="16384" style="5" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A1" s="9">
+    <row r="1" s="7" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A1" s="8">
         <v>1</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" s="10" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A2" s="11">
+        <v>2</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-    </row>
-    <row r="2" s="11" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A2" s="12">
-        <v>2</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" s="10" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A3" s="11">
+        <v>3</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-    </row>
-    <row r="3" s="11" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A3" s="12">
-        <v>3</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="15" t="s">
+      <c r="F3" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" s="10" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A4" s="11">
+        <v>4</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="E4" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-    </row>
-    <row r="4" s="11" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A4" s="12">
-        <v>4</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="E4" s="17" t="s">
+      <c r="F4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" s="10" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A5" s="11">
+        <v>5</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-    </row>
-    <row r="5" s="11" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A5" s="12">
-        <v>5</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="18" t="s">
+      <c r="D5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="18" t="s">
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" s="10" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A6" s="11">
+        <v>6</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="13"/>
-    </row>
-    <row r="6" s="11" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A6" s="12">
-        <v>6</v>
-      </c>
-      <c r="B6" s="17" t="s">
+      <c r="C6" s="12"/>
+      <c r="D6" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="16" t="s">
+      <c r="F6" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="G6" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" s="16" t="s">
+    </row>
+    <row r="7" s="10" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A7" s="11">
+        <v>7</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="17" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" s="11" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A7" s="12">
-        <v>7</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="18" t="s">
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="18" t="s">
+    </row>
+    <row r="8" s="19" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A8" s="20">
+        <v>8</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="22" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="8" s="20" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A8" s="21">
-        <v>8</v>
-      </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="23" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Table header and pagination is shown when table is empty
</commit_message>
<xml_diff>
--- a/Prop destinations.xlsx
+++ b/Prop destinations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Prop</t>
   </si>
@@ -67,6 +67,9 @@
     <t>emptyPlaceholder</t>
   </si>
   <si>
+    <t xml:space="preserve">5 - BodyContainer</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
@@ -88,9 +91,6 @@
     <t xml:space="preserve">5 - HeadContainer</t>
   </si>
   <si>
-    <t xml:space="preserve">5 - BodyContainer</t>
-  </si>
-  <si>
     <t>columnOrder</t>
   </si>
   <si>
@@ -121,6 +121,15 @@
     <t>onKeyDown</t>
   </si>
   <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>itemContainerRef</t>
+  </si>
+  <si>
+    <t>placeholder</t>
+  </si>
+  <si>
     <t>options</t>
   </si>
   <si>
@@ -151,7 +160,7 @@
     <t>columnResizeStart</t>
   </si>
   <si>
-    <t>setResizingColumn</t>
+    <t>setCursorClass</t>
   </si>
   <si>
     <t>isTouching</t>
@@ -206,7 +215,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -251,31 +260,17 @@
       <b/>
       <color theme="1"/>
       <sz val="10"/>
-      <u val="single"/>
     </font>
     <font>
       <name val="Arial"/>
       <b/>
       <color rgb="FF00B050"/>
       <sz val="10"/>
-      <u val="single"/>
     </font>
     <font>
       <name val="Arial"/>
       <b/>
       <color rgb="FF7030A0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <b/>
-      <color theme="1"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <b/>
-      <color rgb="FF00B050"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -343,7 +338,7 @@
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
@@ -381,12 +376,6 @@
     <xf fontId="9" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="10" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="11" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="4" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -396,7 +385,7 @@
     <xf fontId="6" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="10" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="7" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -414,14 +403,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>890583</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>900107</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>676271</xdr:rowOff>
+      <xdr:rowOff>676270</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>623882</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>633406</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>257169</xdr:rowOff>
     </xdr:to>
@@ -435,7 +424,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="5795958" y="1571621"/>
+          <a:off x="7224708" y="1571620"/>
           <a:ext cx="1152524" cy="476249"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -532,16 +521,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>700084</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>709609</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>676271</xdr:rowOff>
+      <xdr:rowOff>676270</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>700084</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>709609</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>238119</xdr:rowOff>
+      <xdr:rowOff>238118</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -553,7 +542,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="5605459" y="676271"/>
+          <a:off x="7034209" y="676270"/>
           <a:ext cx="0" cy="457198"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -709,16 +698,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>823909</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>833434</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>676271</xdr:rowOff>
+      <xdr:rowOff>676270</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>557206</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>566731</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>257169</xdr:rowOff>
+      <xdr:rowOff>257168</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -730,7 +719,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1" flipV="0">
-          <a:off x="4310059" y="1571621"/>
+          <a:off x="5738809" y="1571620"/>
           <a:ext cx="1152522" cy="476248"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -827,124 +816,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>704846</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>676272</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>704846</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>238119</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="11" name="" hidden="0"/>
-        <xdr:cNvCxnSpPr>
-          <a:cxnSpLocks/>
-        </xdr:cNvCxnSpPr>
-        <xdr:nvPr isPhoto="0" userDrawn="0"/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipH="0" flipV="0">
-          <a:off x="7029446" y="2466972"/>
-          <a:ext cx="0" cy="457197"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19049" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter/>
-          <a:tailEnd type="arrow" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>719134</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>666746</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>719134</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>228594</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="12" name="" hidden="0"/>
-        <xdr:cNvCxnSpPr>
-          <a:cxnSpLocks/>
-        </xdr:cNvCxnSpPr>
-        <xdr:nvPr isPhoto="0" userDrawn="0"/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipH="0" flipV="0">
-          <a:off x="5624509" y="1562096"/>
-          <a:ext cx="0" cy="457198"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19049" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter/>
-          <a:tailEnd type="arrow" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>842959</xdr:colOff>
       <xdr:row>4</xdr:row>
@@ -958,7 +829,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="" hidden="0"/>
+        <xdr:cNvPr id="11" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1017,7 +888,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="" hidden="0"/>
+        <xdr:cNvPr id="12" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1076,7 +947,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="" hidden="0"/>
+        <xdr:cNvPr id="13" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1135,7 +1006,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="" hidden="0"/>
+        <xdr:cNvPr id="14" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1194,7 +1065,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="" hidden="0"/>
+        <xdr:cNvPr id="15" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1253,7 +1124,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="18" name="" hidden="0"/>
+        <xdr:cNvPr id="16" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1312,7 +1183,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="19" name="" hidden="0"/>
+        <xdr:cNvPr id="17" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1940,37 +1811,37 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" ht="14.25">
@@ -2027,7 +1898,7 @@
         <v>28</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" ht="14.25">
@@ -2045,7 +1916,7 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" ht="14.25">
@@ -2061,169 +1932,168 @@
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
+      <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" ht="14.25">
-      <c r="A21" t="s">
+      <c r="F22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="C24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" s="2" customFormat="1" ht="14.25">
-      <c r="A22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" ht="14.25">
-      <c r="A23" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25">
-      <c r="A24" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="E24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" s="2" customFormat="1" ht="14.25">
       <c r="A25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="A26" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" ht="14.25">
-      <c r="A26" t="s">
+      <c r="C26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="F26" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" ht="14.25">
-      <c r="A27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" ht="14.25">
-      <c r="A28" t="s">
+      <c r="C27" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" s="2" customFormat="1" ht="14.25">
+      <c r="A28" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>24</v>
+      <c r="B29" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="30" ht="14.25">
@@ -2231,15 +2101,48 @@
         <v>47</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" ht="14.25"/>
-    <row r="36" ht="14.25">
-      <c r="A36" s="2"/>
+    <row r="32" ht="14.25">
+      <c r="A32" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25"/>
+    <row r="39" ht="14.25">
+      <c r="A39" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -2274,10 +2177,9 @@
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
-      <c r="E1" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="9"/>
+      <c r="F1" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
     </row>
@@ -2288,10 +2190,9 @@
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
-      <c r="E2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="12"/>
+      <c r="F2" s="13" t="s">
+        <v>52</v>
+      </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
     </row>
@@ -2301,16 +2202,13 @@
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="D3" s="12"/>
       <c r="E3" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="12"/>
+        <v>53</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>54</v>
+      </c>
       <c r="H3" s="12"/>
     </row>
     <row r="4" s="10" customFormat="1" ht="70.5" customHeight="1">
@@ -2320,11 +2218,9 @@
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="E4" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>13</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="F4" s="12"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
     </row>
@@ -2333,13 +2229,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="17" t="s">
-        <v>53</v>
+      <c r="C5" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="D5" s="12"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="17" t="s">
-        <v>54</v>
+      <c r="G5" s="15" t="s">
+        <v>57</v>
       </c>
       <c r="H5" s="12"/>
     </row>
@@ -2348,20 +2244,20 @@
         <v>6</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>60</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" s="10" customFormat="1" ht="70.5" customHeight="1">
@@ -2370,26 +2266,26 @@
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
-      <c r="D7" s="17" t="s">
-        <v>59</v>
+      <c r="D7" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
-      <c r="H7" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" s="19" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A8" s="20">
+      <c r="H7" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" s="17" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A8" s="18">
         <v>8</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="22" t="s">
-        <v>61</v>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added index validation in all action handlers
</commit_message>
<xml_diff>
--- a/Prop destinations.xlsx
+++ b/Prop destinations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Prop</t>
   </si>
@@ -164,6 +164,24 @@
   </si>
   <si>
     <t>scrollToPos</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 - Pagination</t>
+  </si>
+  <si>
+    <t>pageCount</t>
+  </si>
+  <si>
+    <t>goToPage</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 - Error</t>
   </si>
   <si>
     <t>Connector</t>
@@ -393,6 +411,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -429,11 +452,9 @@
         </a:prstGeom>
         <a:ln w="19049" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+            <a:srgbClr val="43739E"/>
           </a:solidFill>
-          <a:prstDash val="solid"/>
+          <a:prstDash val="sysDash"/>
           <a:miter/>
           <a:tailEnd type="arrow" len="med"/>
         </a:ln>
@@ -519,15 +540,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>709609</xdr:colOff>
+      <xdr:colOff>728658</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>676270</xdr:rowOff>
+      <xdr:rowOff>676269</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>709609</xdr:colOff>
+      <xdr:colOff>728658</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>238118</xdr:rowOff>
+      <xdr:rowOff>238117</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -539,7 +560,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="7034209" y="676270"/>
+          <a:off x="7053258" y="676269"/>
           <a:ext cx="0" cy="457198"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -665,11 +686,9 @@
         </a:prstGeom>
         <a:ln w="19049" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+            <a:srgbClr val="43739E"/>
           </a:solidFill>
-          <a:prstDash val="solid"/>
+          <a:prstDash val="sysDash"/>
           <a:miter/>
           <a:tailEnd type="arrow" len="med"/>
         </a:ln>
@@ -1109,15 +1128,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>714373</xdr:colOff>
+      <xdr:colOff>733422</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>666747</xdr:rowOff>
+      <xdr:rowOff>657221</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>714373</xdr:colOff>
+      <xdr:colOff>733422</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>228595</xdr:rowOff>
+      <xdr:rowOff>219068</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -1129,7 +1148,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="8458198" y="4248147"/>
+          <a:off x="8477247" y="4238621"/>
           <a:ext cx="0" cy="457197"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1137,11 +1156,9 @@
         </a:prstGeom>
         <a:ln w="19049" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+            <a:srgbClr val="43739E"/>
           </a:solidFill>
-          <a:prstDash val="solid"/>
+          <a:prstDash val="sysDash"/>
           <a:miter/>
           <a:tailEnd type="arrow" len="med"/>
         </a:ln>
@@ -1190,6 +1207,122 @@
         <a:xfrm flipH="1" flipV="0">
           <a:off x="2995607" y="3362321"/>
           <a:ext cx="2466973" cy="485773"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19049" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter/>
+          <a:tailEnd type="arrow" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>728658</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>676269</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>728658</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>238116</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="" hidden="0"/>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+        </xdr:cNvCxnSpPr>
+        <xdr:nvPr isPhoto="0" userDrawn="0"/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="7053258" y="1571619"/>
+          <a:ext cx="0" cy="457196"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19049" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="43739E"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:miter/>
+          <a:tailEnd type="arrow" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>714372</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>676271</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>714372</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>238118</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="" hidden="0"/>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+        </xdr:cNvCxnSpPr>
+        <xdr:nvPr isPhoto="0" userDrawn="0"/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="8458197" y="2466971"/>
+          <a:ext cx="0" cy="457196"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1726,12 +1859,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="29.00390625"/>
-    <col customWidth="1" min="3" max="3" width="29.7109375"/>
-    <col customWidth="1" min="4" max="4" width="29.28125"/>
-    <col customWidth="1" min="5" max="5" width="28.00390625"/>
-    <col customWidth="1" min="6" max="7" width="27.8515625"/>
-    <col min="8" max="16384" width="9.140625"/>
+    <col bestFit="1" customWidth="1" min="1" max="2" width="29.00390625"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" width="29.7109375"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" width="29.28125"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" width="28.00390625"/>
+    <col bestFit="1" customWidth="1" min="6" max="7" width="27.8515625"/>
+    <col bestFit="1" min="8" max="16384" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="18.75">
@@ -2132,6 +2265,50 @@
       </c>
       <c r="C33" s="2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25">
+      <c r="A34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="A36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="A37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="38" ht="14.25"/>
@@ -2159,9 +2336,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" style="6" width="9.7109375"/>
-    <col customWidth="1" min="2" max="8" style="5" width="21.28125"/>
-    <col min="9" max="16384" style="5" width="9.140625"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="6" width="9.7109375"/>
+    <col bestFit="1" customWidth="1" min="2" max="8" style="5" width="21.28125"/>
+    <col bestFit="1" min="9" max="16384" style="5" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="1" ht="70.5" customHeight="1">
@@ -2172,7 +2349,7 @@
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="F1" s="9" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
@@ -2185,7 +2362,7 @@
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="F2" s="13" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -2198,10 +2375,13 @@
       <c r="C3" s="10"/>
       <c r="D3" s="12"/>
       <c r="E3" s="14" t="s">
-        <v>52</v>
+        <v>58</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="H3" s="12"/>
     </row>
@@ -2212,10 +2392,12 @@
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="E4" s="16" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="G4" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="H4" s="12"/>
     </row>
     <row r="5" s="10" customFormat="1" ht="70.5" customHeight="1">
@@ -2224,12 +2406,12 @@
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="15" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="15" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="H5" s="12"/>
     </row>
@@ -2238,20 +2420,20 @@
         <v>6</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="15" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" s="10" customFormat="1" ht="70.5" customHeight="1">
@@ -2261,12 +2443,12 @@
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="15" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="15" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" s="17" customFormat="1" ht="70.5" customHeight="1">
@@ -2279,7 +2461,7 @@
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
       <c r="H8" s="20" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wrapped table and body placeholders into div
</commit_message>
<xml_diff>
--- a/Prop destinations.xlsx
+++ b/Prop destinations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Prop</t>
   </si>
@@ -52,60 +52,60 @@
     <t>Error</t>
   </si>
   <si>
+    <t xml:space="preserve">3 - ScrollingContainer</t>
+  </si>
+  <si>
+    <t>Pagination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 - PaginationContainer</t>
+  </si>
+  <si>
+    <t>loadingIndicator</t>
+  </si>
+  <si>
+    <t>emptyPlaceholder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 - BodyContainer</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 - TableHead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 - TableBody</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 - ColumnGroup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 - TableRow</t>
+  </si>
+  <si>
+    <t>className</t>
+  </si>
+  <si>
+    <t>columnOrder</t>
+  </si>
+  <si>
+    <t>initColumnWidths</t>
+  </si>
+  <si>
+    <t>showSelectionRect</t>
+  </si>
+  <si>
+    <t>scrollFactor</t>
+  </si>
+  <si>
+    <t>onContextMenu</t>
+  </si>
+  <si>
     <t xml:space="preserve">2 - Root</t>
   </si>
   <si>
-    <t>Pagination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 - PaginationContainer</t>
-  </si>
-  <si>
-    <t>loadingIndicator</t>
-  </si>
-  <si>
-    <t>emptyPlaceholder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 - BodyContainer</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 - TableHead</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 - TableBody</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 - ColumnGroup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 - TableRow</t>
-  </si>
-  <si>
-    <t>className</t>
-  </si>
-  <si>
-    <t>columnOrder</t>
-  </si>
-  <si>
-    <t>initColumnWidths</t>
-  </si>
-  <si>
-    <t>showSelectionRect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 - ScrollingContainer</t>
-  </si>
-  <si>
-    <t>scrollFactor</t>
-  </si>
-  <si>
-    <t>onContextMenu</t>
-  </si>
-  <si>
     <t>onItemsOpen</t>
   </si>
   <si>
@@ -124,13 +124,10 @@
     <t>itemContainerRef</t>
   </si>
   <si>
-    <t>placeholder</t>
-  </si>
-  <si>
     <t>storage</t>
   </si>
   <si>
-    <t>dispatchers</t>
+    <t>actions</t>
   </si>
   <si>
     <t xml:space="preserve">7 - TableHeader</t>
@@ -1931,7 +1928,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1995,25 +1992,25 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" ht="14.25">
@@ -2022,7 +2019,7 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>17</v>
@@ -2034,7 +2031,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" ht="14.25">
@@ -2052,10 +2049,10 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="19" ht="14.25">
@@ -2074,28 +2071,39 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>12</v>
+      <c r="B21" t="s">
+        <v>8</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" ht="14.25">
       <c r="A22" t="s">
         <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>12</v>
@@ -2104,109 +2112,100 @@
         <v>14</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" s="2" customFormat="1" ht="14.25">
+      <c r="A24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="A25" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="C25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" s="2" customFormat="1" ht="14.25">
-      <c r="A25" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="E25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="26" ht="14.25">
       <c r="A26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" s="2" customFormat="1" ht="14.25">
+      <c r="A27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="4" t="s">
+    </row>
+    <row r="28" ht="14.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" ht="14.25">
-      <c r="A27" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" s="2" customFormat="1" ht="14.25">
-      <c r="A28" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>42</v>
+      <c r="D28" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="29" ht="14.25">
@@ -2214,13 +2213,10 @@
         <v>45</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" ht="14.25">
@@ -2228,32 +2224,32 @@
         <v>46</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" t="s">
+      <c r="A31" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>27</v>
+      <c r="B31" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="A32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="32" ht="14.25">
-      <c r="A32" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="33" ht="14.25">
@@ -2261,21 +2257,21 @@
         <v>49</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" ht="14.25">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" ht="14.25">
@@ -2286,7 +2282,7 @@
         <v>14</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" ht="14.25">
@@ -2294,26 +2290,15 @@
         <v>53</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" ht="14.25">
-      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" ht="14.25"/>
-    <row r="39" ht="14.25">
-      <c r="A39" s="2"/>
+    </row>
+    <row r="37" ht="14.25"/>
+    <row r="38" ht="14.25">
+      <c r="A38" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -2349,7 +2334,7 @@
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="F1" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
@@ -2362,7 +2347,7 @@
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="F2" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -2375,13 +2360,13 @@
       <c r="C3" s="10"/>
       <c r="D3" s="12"/>
       <c r="E3" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H3" s="12"/>
     </row>
@@ -2392,7 +2377,7 @@
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="E4" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12" t="s">
@@ -2406,12 +2391,12 @@
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="12"/>
     </row>
@@ -2420,20 +2405,20 @@
         <v>6</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="G6" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="15" t="s">
         <v>65</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="7" s="10" customFormat="1" ht="70.5" customHeight="1">
@@ -2443,12 +2428,12 @@
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" s="17" customFormat="1" ht="70.5" customHeight="1">
@@ -2461,7 +2446,7 @@
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
       <c r="H8" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Focus is now retained when changing pages
</commit_message>
<xml_diff>
--- a/Prop destinations.xlsx
+++ b/Prop destinations.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Props" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,27 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
-  <si>
-    <t>Prop</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+  <si>
+    <t>Name</t>
   </si>
   <si>
     <t>Source</t>
   </si>
   <si>
-    <t xml:space="preserve">Destination 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Destination 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Destination 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Destination 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Destination 5</t>
+    <t>Destinations</t>
   </si>
   <si>
     <t>namespace</t>
@@ -88,6 +76,9 @@
     <t>className</t>
   </si>
   <si>
+    <t xml:space="preserve">2 - Root</t>
+  </si>
+  <si>
     <t>columnOrder</t>
   </si>
   <si>
@@ -103,9 +94,6 @@
     <t>onContextMenu</t>
   </si>
   <si>
-    <t xml:space="preserve">2 - Root</t>
-  </si>
-  <si>
     <t>onItemsOpen</t>
   </si>
   <si>
@@ -179,6 +167,21 @@
   </si>
   <si>
     <t xml:space="preserve">3 - Error</t>
+  </si>
+  <si>
+    <t>showPlaceholder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Context provider</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ref setter</t>
+  </si>
+  <si>
+    <t>Override</t>
   </si>
   <si>
     <t>Connector</t>
@@ -286,7 +289,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +306,42 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor theme="5" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor theme="7" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor theme="6" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor theme="5" tint="0.59999389629810485"/>
       </patternFill>
     </fill>
     <fill/>
@@ -345,17 +384,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="3" applyFill="1"/>
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="5" applyFill="1"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="6" applyFill="1"/>
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="4" applyFill="1"/>
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="49" xfId="4" applyNumberFormat="1" applyFill="1"/>
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="5" applyFill="1"/>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -376,7 +431,7 @@
     <xf fontId="6" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="7" fillId="4" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="7" fillId="10" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="8" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -401,10 +456,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+    <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
+    <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
+    <cellStyle name="20% - Accent6" xfId="5" builtinId="50"/>
+    <cellStyle name="20% - Accent4" xfId="6" builtinId="42"/>
+    <cellStyle name="20% - Accent3" xfId="7" builtinId="38"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -420,16 +481,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>900107</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>890581</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>676270</xdr:rowOff>
+      <xdr:rowOff>676269</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>633406</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>623880</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>257169</xdr:rowOff>
+      <xdr:rowOff>257168</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -441,7 +502,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="7224708" y="1571620"/>
+          <a:off x="5795956" y="1571619"/>
           <a:ext cx="1152524" cy="476249"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -451,7 +512,7 @@
           <a:solidFill>
             <a:srgbClr val="43739E"/>
           </a:solidFill>
-          <a:prstDash val="sysDash"/>
+          <a:prstDash val="solid"/>
           <a:miter/>
           <a:tailEnd type="arrow" len="med"/>
         </a:ln>
@@ -536,16 +597,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>728658</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>709608</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>676269</xdr:rowOff>
+      <xdr:rowOff>676268</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>728658</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>709608</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>238117</xdr:rowOff>
+      <xdr:rowOff>238116</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -557,7 +618,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="7053258" y="676269"/>
+          <a:off x="5614983" y="676268"/>
           <a:ext cx="0" cy="457198"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -595,65 +656,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>700084</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>676272</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>700084</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>238120</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="" hidden="0"/>
-        <xdr:cNvCxnSpPr>
-          <a:cxnSpLocks/>
-        </xdr:cNvCxnSpPr>
-        <xdr:nvPr isPhoto="0" userDrawn="0"/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipH="0" flipV="0">
-          <a:off x="5605459" y="2466972"/>
-          <a:ext cx="0" cy="457198"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19049" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter/>
-          <a:tailEnd type="arrow" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>866774</xdr:colOff>
       <xdr:row>4</xdr:row>
@@ -667,7 +669,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="8" name="" hidden="0"/>
+        <xdr:cNvPr id="7" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -711,20 +713,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>833434</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>823908</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>676270</xdr:rowOff>
+      <xdr:rowOff>676269</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>566731</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>557205</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>257168</xdr:rowOff>
+      <xdr:rowOff>257167</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="" hidden="0"/>
+        <xdr:cNvPr id="8" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -732,7 +734,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1" flipV="0">
-          <a:off x="5738809" y="1571620"/>
+          <a:off x="4310058" y="1571619"/>
           <a:ext cx="1152522" cy="476248"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -783,7 +785,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="" hidden="0"/>
+        <xdr:cNvPr id="9" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -842,7 +844,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="11" name="" hidden="0"/>
+        <xdr:cNvPr id="10" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -901,7 +903,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="12" name="" hidden="0"/>
+        <xdr:cNvPr id="11" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -960,7 +962,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="" hidden="0"/>
+        <xdr:cNvPr id="12" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1019,7 +1021,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="" hidden="0"/>
+        <xdr:cNvPr id="13" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1078,7 +1080,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="" hidden="0"/>
+        <xdr:cNvPr id="14" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1137,7 +1139,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="" hidden="0"/>
+        <xdr:cNvPr id="15" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1194,7 +1196,7 @@
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="" hidden="0"/>
+        <xdr:cNvPr id="16" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1241,19 +1243,19 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>728658</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>676269</xdr:rowOff>
+      <xdr:colOff>723896</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>676271</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>728658</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>238116</xdr:rowOff>
+      <xdr:colOff>723896</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>238117</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="18" name="" hidden="0"/>
+        <xdr:cNvPr id="17" name="" hidden="0"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
         </xdr:cNvCxnSpPr>
@@ -1261,7 +1263,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="7053258" y="1571619"/>
+          <a:off x="7048496" y="2466971"/>
           <a:ext cx="0" cy="457196"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1297,16 +1299,73 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>714372</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>890583</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>676271</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>714372</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>623882</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>238118</xdr:rowOff>
+      <xdr:rowOff>257170</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="" hidden="0"/>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+        </xdr:cNvCxnSpPr>
+        <xdr:nvPr isPhoto="0" userDrawn="0"/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="4376733" y="2466971"/>
+          <a:ext cx="1152523" cy="476248"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19049" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="43739E"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter/>
+          <a:tailEnd type="arrow" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>823910</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>676271</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>557207</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>257169</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -1317,20 +1376,18 @@
         <xdr:nvPr isPhoto="0" userDrawn="0"/>
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
-        <a:xfrm flipH="0" flipV="0">
-          <a:off x="8458197" y="2466971"/>
-          <a:ext cx="0" cy="457196"/>
+        <a:xfrm flipH="1" flipV="0">
+          <a:off x="2890835" y="2466971"/>
+          <a:ext cx="1152522" cy="476247"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="19049" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+            <a:srgbClr val="43739E"/>
           </a:solidFill>
-          <a:prstDash val="solid"/>
+          <a:prstDash val="sysDash"/>
           <a:miter/>
           <a:tailEnd type="arrow" len="med"/>
         </a:ln>
@@ -1865,442 +1922,480 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="18.75">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="B2" s="4"/>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="B3" s="4"/>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="B5" s="4"/>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2" t="s">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25">
-      <c r="A14" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" ht="14.25">
-      <c r="A15" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25">
-      <c r="A16" t="s">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" ht="14.25">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25">
-      <c r="A19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" ht="14.25">
-      <c r="A20" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="2"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" ht="14.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22" ht="14.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" s="2" customFormat="1" ht="14.25">
-      <c r="A24" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" s="4" customFormat="1" ht="14.25">
+      <c r="A24" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
     </row>
     <row r="25" ht="14.25">
       <c r="A25" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>17</v>
+        <v>8</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>20</v>
+        <v>37</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="26" ht="14.25">
       <c r="A26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" s="4" customFormat="1" ht="14.25">
+      <c r="A27" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="A28" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="A29" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25">
+      <c r="A30" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" s="2" customFormat="1" ht="14.25">
-      <c r="A27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" ht="14.25">
-      <c r="A28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" ht="14.25">
-      <c r="A29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" ht="14.25">
-      <c r="A30" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>10</v>
+      <c r="B30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="31" ht="14.25">
       <c r="A31" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>10</v>
+      <c r="A32" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="33" ht="14.25">
       <c r="A33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="34" ht="14.25">
       <c r="A34" t="s">
-        <v>51</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="35" ht="14.25">
-      <c r="A35" t="s">
-        <v>52</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>50</v>
+      <c r="A35" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="36" ht="14.25">
       <c r="A36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="A38" s="4"/>
+    </row>
+    <row r="44" ht="14.25">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45" ht="14.25">
+      <c r="A45" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" ht="14.25">
+      <c r="A46" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="47" ht="14.25">
+      <c r="A47" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="37" ht="14.25"/>
-    <row r="38" ht="14.25">
-      <c r="A38" s="2"/>
+    <row r="48" ht="14.25">
+      <c r="A48" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:G1"/>
+  </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
@@ -2321,132 +2416,130 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" style="6" width="9.7109375"/>
-    <col bestFit="1" customWidth="1" min="2" max="8" style="5" width="21.28125"/>
-    <col bestFit="1" min="9" max="16384" style="5" width="9.140625"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="12" width="9.7109375"/>
+    <col bestFit="1" customWidth="1" min="2" max="8" style="11" width="21.28125"/>
+    <col bestFit="1" min="9" max="16384" style="11" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A1" s="8">
+    <row r="1" s="13" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A1" s="14">
         <v>1</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="F1" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-    </row>
-    <row r="2" s="10" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A2" s="11">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="15"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" s="16" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A2" s="17">
         <v>2</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="F2" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-    </row>
-    <row r="3" s="10" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A3" s="11">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="18"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="3" s="16" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A3" s="17">
         <v>3</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="15" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="12"/>
-    </row>
-    <row r="4" s="10" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A4" s="11">
+      <c r="E3" s="18"/>
+      <c r="F3" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" s="16" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A4" s="17">
         <v>4</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="E4" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="12"/>
-    </row>
-    <row r="5" s="10" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A5" s="11">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" s="16" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A5" s="17">
         <v>5</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="15" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="H5" s="12"/>
-    </row>
-    <row r="6" s="10" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A6" s="11">
+      <c r="D5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" s="16" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A6" s="17">
         <v>6</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="15" t="s">
+      <c r="B6" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="15" t="s">
+      <c r="F6" s="20" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" s="10" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A7" s="11">
+      <c r="G6" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" s="16" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A7" s="17">
         <v>7</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="15" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="21" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="8" s="17" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A8" s="18">
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" s="23" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A8" s="24">
         <v>8</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="20" t="s">
-        <v>68</v>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved keyboard navigation when using pagination
</commit_message>
<xml_diff>
--- a/Prop destinations.xlsx
+++ b/Prop destinations.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Props" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>autoFocus</t>
   </si>
   <si>
     <t>itemContainerRef</t>
@@ -395,22 +398,19 @@
     <xf fontId="0" fillId="8" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="0" fillId="9" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="3" applyFill="1"/>
     <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="5" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="6" applyFill="1"/>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="4" applyFill="1"/>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="49" xfId="4" applyNumberFormat="1" applyFill="1"/>
-    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="5" applyFill="1"/>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -469,11 +469,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -482,13 +477,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>890581</xdr:colOff>
+      <xdr:colOff>890580</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>676269</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>623880</xdr:colOff>
+      <xdr:colOff>623879</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>257168</xdr:rowOff>
     </xdr:to>
@@ -618,7 +613,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="5614983" y="676268"/>
+          <a:off x="5614982" y="676268"/>
           <a:ext cx="0" cy="457198"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -722,7 +717,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>557205</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>257167</xdr:rowOff>
+      <xdr:rowOff>257166</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -1308,7 +1303,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>623882</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>257170</xdr:rowOff>
+      <xdr:rowOff>257169</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -1357,7 +1352,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>823910</xdr:colOff>
+      <xdr:colOff>823909</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>676271</xdr:rowOff>
     </xdr:from>
@@ -1928,19 +1923,19 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="3"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -1949,7 +1944,7 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="3"/>
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -1958,8 +1953,8 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1967,7 +1962,7 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="3"/>
       <c r="C5" t="s">
         <v>10</v>
       </c>
@@ -1976,8 +1971,8 @@
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1985,8 +1980,8 @@
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1994,14 +1989,14 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F8" t="s">
@@ -2015,8 +2010,8 @@
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2024,8 +2019,8 @@
       <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2033,8 +2028,8 @@
       <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2042,8 +2037,8 @@
       <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2051,345 +2046,355 @@
       <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="4"/>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="4"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="4"/>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" t="s">
+      <c r="A21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" ht="14.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
       <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>18</v>
+      <c r="E22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" s="4" customFormat="1" ht="14.25">
-      <c r="A24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="8" t="s">
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" s="3" customFormat="1" ht="14.25">
+      <c r="A25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" ht="14.25">
-      <c r="A25" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="A26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" ht="14.25">
-      <c r="A26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" t="s">
-        <v>8</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" s="4" customFormat="1" ht="14.25">
-      <c r="A27" s="4" t="s">
+      <c r="E26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" ht="14.25">
-      <c r="A28" s="6" t="s">
+      <c r="D27" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" s="3" customFormat="1" ht="14.25">
+      <c r="A28" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="A29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" ht="14.25">
-      <c r="A29" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="4" t="s">
+    <row r="30" ht="14.25">
+      <c r="A30" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" ht="14.25">
-      <c r="A30" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="A31" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" ht="14.25">
-      <c r="A31" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="7" t="s">
+    <row r="32" ht="14.25">
+      <c r="A32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" ht="14.25">
-      <c r="A32" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="4" t="s">
+    <row r="33" ht="14.25">
+      <c r="A33" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="33" ht="14.25">
-      <c r="A33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="34" ht="14.25">
       <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="4" t="s">
+    </row>
+    <row r="35" ht="14.25">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" ht="14.25">
-      <c r="A35" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="4" t="s">
+      <c r="C35" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="A36" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" ht="14.25">
-      <c r="A36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" t="s">
-        <v>50</v>
+      <c r="C36" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="37" ht="14.25">
       <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="4" t="s">
+    </row>
+    <row r="38" ht="14.25">
+      <c r="A38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D38" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" ht="14.25">
-      <c r="A38" s="4"/>
-    </row>
-    <row r="44" ht="14.25">
-      <c r="A44" s="4"/>
+    <row r="39" ht="14.25">
+      <c r="A39" s="3"/>
     </row>
     <row r="45" ht="14.25">
-      <c r="A45" s="9" t="s">
-        <v>52</v>
-      </c>
+      <c r="A45" s="3"/>
     </row>
     <row r="46" ht="14.25">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="9" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="47" ht="14.25">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="48" ht="14.25">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="7" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="49" ht="14.25">
+      <c r="A49" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2416,130 +2421,130 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" style="12" width="9.7109375"/>
-    <col bestFit="1" customWidth="1" min="2" max="8" style="11" width="21.28125"/>
-    <col bestFit="1" min="9" max="16384" style="11" width="9.140625"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="11" width="9.7109375"/>
+    <col bestFit="1" customWidth="1" min="2" max="8" style="10" width="21.28125"/>
+    <col bestFit="1" min="9" max="16384" style="10" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" s="13" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A1" s="14">
+    <row r="1" s="12" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A1" s="13">
         <v>1</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="15"/>
-      <c r="H1" s="15"/>
-    </row>
-    <row r="2" s="16" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A2" s="17">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" s="15" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A2" s="16">
         <v>2</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="18"/>
-      <c r="H2" s="18"/>
-    </row>
-    <row r="3" s="16" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A3" s="17">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="H2" s="17"/>
+    </row>
+    <row r="3" s="15" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A3" s="16">
         <v>3</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="21" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="18"/>
-    </row>
-    <row r="4" s="16" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A4" s="17">
+      <c r="E3" s="17"/>
+      <c r="F3" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="17"/>
+    </row>
+    <row r="4" s="15" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A4" s="16">
         <v>4</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="18" t="s">
+      <c r="E4" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="18"/>
-    </row>
-    <row r="5" s="16" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A5" s="17">
+      <c r="H4" s="17"/>
+    </row>
+    <row r="5" s="15" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A5" s="16">
         <v>5</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="21" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="18"/>
-    </row>
-    <row r="6" s="16" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A6" s="17">
+      <c r="D5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="17"/>
+    </row>
+    <row r="6" s="15" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A6" s="16">
         <v>6</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="21" t="s">
+      <c r="B6" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="C6" s="17"/>
+      <c r="D6" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" s="21" t="s">
+      <c r="F6" s="19" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="7" s="16" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A7" s="17">
+      <c r="G6" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" s="15" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A7" s="16">
         <v>7</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="21" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="20" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="8" s="23" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A8" s="24">
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" s="22" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A8" s="23">
         <v>8</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26" t="s">
-        <v>69</v>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>